<commit_message>
No se que onda esto
</commit_message>
<xml_diff>
--- a/Mediciones Notch.xlsx
+++ b/Mediciones Notch.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="381" documentId="8_{EFBC0B77-B65F-41DB-A976-CCCD59113E8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5AB9F681-DB90-4F2D-A8EB-BA119EA90903}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4CFCF759-8B86-476F-AAAF-E5A881D45B24}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CFCF759-8B86-476F-AAAF-E5A881D45B24}"/>
   </bookViews>
   <sheets>
     <sheet name="Bode" sheetId="1" r:id="rId1"/>
@@ -29119,7 +29119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C52036-615C-4221-826B-33D52CC39257}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -30236,7 +30236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7E0978-2D75-4D6A-85BE-677DBF9100AD}">
   <dimension ref="A1:K1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K350" sqref="G350:K350"/>
     </sheetView>
   </sheetViews>

</xml_diff>